<commit_message>
1- Added .NET Core - webapi 2- Added GO Fasthttp and Fiber web servers 3- Updated results.txt and comparison.xlsx
</commit_message>
<xml_diff>
--- a/webservers/comparison.xlsx
+++ b/webservers/comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\github.com\gsainz\autocannon\webservers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A30241C5-E3F3-4A92-8859-15A41A32B4EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF5ACCC-30D6-4F6A-BBFE-6A52FBFC6AB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{4D9F741E-112C-4F17-A62D-9BB75CA402CB}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{4D9F741E-112C-4F17-A62D-9BB75CA402CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Web Servers" sheetId="1" r:id="rId1"/>
@@ -35,22 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
-  <si>
-    <t>GIN</t>
-  </si>
-  <si>
-    <t>CHI</t>
-  </si>
-  <si>
-    <t>AIRBORNE</t>
-  </si>
-  <si>
-    <t>ECHO</t>
-  </si>
-  <si>
-    <t>GORILLA</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>NODE</t>
   </si>
@@ -107,6 +92,128 @@
   </si>
   <si>
     <t>Language</t>
+  </si>
+  <si>
+    <t>C#</t>
+  </si>
+  <si>
+    <t>467 MB</t>
+  </si>
+  <si>
+    <t>118 MB</t>
+  </si>
+  <si>
+    <t>94 MB</t>
+  </si>
+  <si>
+    <t>386 MB</t>
+  </si>
+  <si>
+    <t>104 MB</t>
+  </si>
+  <si>
+    <t>490 MB</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">GIN </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>HTTP/1.1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CHI </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>HTTP/1.1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">AIRBORNE </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>HTTP/1.1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ECHO </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>HTTP/1.1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">GORILLA </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>HTTP/1.1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">FASTHTTP </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>HTTP/2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">FIBER </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>HTTP/1.1</t>
+    </r>
+  </si>
+  <si>
+    <t>.NET Core-web.api</t>
   </si>
 </sst>
 </file>
@@ -122,12 +229,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9.8000000000000007"/>
-      <color rgb="FF080808"/>
-      <name val="Courier New"/>
-      <family val="3"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FF080808"/>
       <name val="Courier New"/>
@@ -135,6 +236,12 @@
     </font>
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <color theme="1"/>
       <name val="Courier New"/>
       <family val="3"/>
@@ -154,7 +261,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -203,14 +310,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -218,35 +336,35 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -562,179 +680,240 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{140D5A91-2AEB-442F-9A05-CF626597CC11}">
-  <dimension ref="B2:G12"/>
+  <dimension ref="B2:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" style="12" customWidth="1"/>
     <col min="5" max="5" width="22.5703125" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" customWidth="1"/>
+    <col min="6" max="6" width="24.85546875" style="12" customWidth="1"/>
     <col min="7" max="7" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+    </row>
+    <row r="3" spans="2:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="8"/>
+    </row>
+    <row r="4" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="2">
+        <v>40225</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="1">
+        <v>34487</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="13"/>
+      <c r="C5" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="1">
+        <v>356794</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1220567</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="13"/>
+      <c r="C6" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="1">
+        <v>347713</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1468844</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="13"/>
+      <c r="C7" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="1">
+        <v>363394</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1186377</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="13"/>
+      <c r="C8" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="1">
+        <v>293456</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1025507</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="13"/>
+      <c r="C9" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="1">
+        <v>833419</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="1">
+        <v>3315075</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="10"/>
+      <c r="C10" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="1">
+        <v>779610</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="1">
+        <v>3188453</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-    </row>
-    <row r="3" spans="2:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="12"/>
-    </row>
-    <row r="4" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="9" t="s">
+    </row>
+    <row r="11" spans="2:7" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="2:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="5">
-        <v>40225</v>
-      </c>
-      <c r="E4" s="6" t="s">
+      <c r="D12" s="1">
+        <v>59751</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="2">
-        <v>34487</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="4"/>
-      <c r="C5" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="2">
-        <v>356794</v>
-      </c>
-      <c r="E5" s="6" t="s">
+      <c r="F12" s="1">
+        <v>58416</v>
+      </c>
+      <c r="G12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="2">
-        <v>1220567</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="4"/>
-      <c r="C6" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="2">
-        <v>347713</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="2">
-        <v>1468844</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="4"/>
-      <c r="C7" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="2">
-        <v>363394</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="2">
-        <v>1186377</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="4"/>
-      <c r="C8" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="2">
-        <v>293456</v>
-      </c>
-      <c r="E8" s="6" t="s">
+    </row>
+    <row r="13" spans="2:7" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14" spans="2:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="2">
-        <v>1025507</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-    </row>
-    <row r="10" spans="2:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="3">
-        <v>59751</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="3">
-        <v>58416</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="1"/>
+      <c r="C14" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="1">
+        <v>167410</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="1">
+        <v>784636</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="D2:G2"/>
     <mergeCell ref="F3:G3"/>
-    <mergeCell ref="B4:B8"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
+    <mergeCell ref="B4:B10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
All servers to return the same json payload for valid load tests.
</commit_message>
<xml_diff>
--- a/webservers/comparison.xlsx
+++ b/webservers/comparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\github.com\gsainz\autocannon\webservers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{171C8C9C-2A80-4B44-BEDA-3A0137FA0CE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D181679B-8E4D-4A62-870E-276B53E329D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{4D9F741E-112C-4F17-A62D-9BB75CA402CB}"/>
   </bookViews>
@@ -391,6 +391,39 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -402,39 +435,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -753,7 +753,7 @@
   <dimension ref="B2:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -767,28 +767,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="14" t="s">
+      <c r="C2" s="22"/>
+      <c r="D2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
     </row>
     <row r="3" spans="2:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="12"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="14" t="s">
+      <c r="B3" s="23"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14" t="s">
+      <c r="E3" s="20"/>
+      <c r="F3" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="14"/>
+      <c r="G3" s="20"/>
     </row>
     <row r="4" spans="2:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="s">
@@ -811,187 +811,187 @@
       </c>
     </row>
     <row r="5" spans="2:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="12" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="2">
-        <v>348371</v>
+        <v>241680</v>
       </c>
       <c r="E5" s="3">
-        <v>40</v>
+        <v>127</v>
       </c>
       <c r="F5" s="1">
-        <v>983504</v>
+        <v>706845</v>
       </c>
       <c r="G5" s="3">
-        <v>113</v>
+        <v>372</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B6" s="20"/>
-      <c r="C6" s="18" t="s">
+      <c r="B6" s="18"/>
+      <c r="C6" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="15">
-        <v>356794</v>
-      </c>
-      <c r="E6" s="16">
-        <v>42</v>
-      </c>
-      <c r="F6" s="15">
-        <v>1220567</v>
-      </c>
-      <c r="G6" s="16">
-        <v>145</v>
+      <c r="D6" s="10">
+        <v>270804</v>
+      </c>
+      <c r="E6" s="11">
+        <v>112</v>
+      </c>
+      <c r="F6" s="10">
+        <v>939506</v>
+      </c>
+      <c r="G6" s="11">
+        <v>387</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B7" s="20"/>
-      <c r="C7" s="17" t="s">
+      <c r="B7" s="18"/>
+      <c r="C7" s="12" t="s">
         <v>15</v>
       </c>
       <c r="D7" s="1">
-        <v>347713</v>
+        <v>262366</v>
       </c>
       <c r="E7" s="3">
-        <v>41</v>
+        <v>157</v>
       </c>
       <c r="F7" s="1">
-        <v>1468844</v>
+        <v>743553</v>
       </c>
       <c r="G7" s="3">
-        <v>175</v>
+        <v>446</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B8" s="20"/>
-      <c r="C8" s="17" t="s">
+      <c r="B8" s="18"/>
+      <c r="C8" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D8" s="1">
-        <v>363394</v>
+        <v>249728</v>
       </c>
       <c r="E8" s="3">
-        <v>42</v>
+        <v>132</v>
       </c>
       <c r="F8" s="1">
-        <v>1186377</v>
+        <v>849918</v>
       </c>
       <c r="G8" s="3">
-        <v>138</v>
+        <v>472</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B9" s="20"/>
-      <c r="C9" s="17" t="s">
+      <c r="B9" s="18"/>
+      <c r="C9" s="12" t="s">
         <v>17</v>
       </c>
       <c r="D9" s="1">
-        <v>293456</v>
+        <v>233067</v>
       </c>
       <c r="E9" s="3">
-        <v>35</v>
+        <v>96</v>
       </c>
       <c r="F9" s="1">
-        <v>1025507</v>
+        <v>888242</v>
       </c>
       <c r="G9" s="3">
-        <v>122</v>
+        <v>366</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B10" s="20"/>
-      <c r="C10" s="17" t="s">
+      <c r="B10" s="18"/>
+      <c r="C10" s="12" t="s">
         <v>18</v>
       </c>
       <c r="D10" s="1">
-        <v>833419</v>
+        <v>577112</v>
       </c>
       <c r="E10" s="3">
-        <v>118</v>
+        <v>248</v>
       </c>
       <c r="F10" s="1">
-        <v>3315075</v>
+        <v>1779269</v>
       </c>
       <c r="G10" s="3">
-        <v>467</v>
+        <v>765</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B11" s="21"/>
-      <c r="C11" s="18" t="s">
+      <c r="B11" s="19"/>
+      <c r="C11" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="15">
-        <v>779610</v>
-      </c>
-      <c r="E11" s="16">
-        <v>94</v>
-      </c>
-      <c r="F11" s="15">
-        <v>3188453</v>
-      </c>
-      <c r="G11" s="16">
-        <v>386</v>
+      <c r="D11" s="10">
+        <v>554514</v>
+      </c>
+      <c r="E11" s="11">
+        <v>284</v>
+      </c>
+      <c r="F11" s="10">
+        <v>1571096</v>
+      </c>
+      <c r="G11" s="11">
+        <v>804</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="22"/>
-      <c r="C12" s="22"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
       <c r="D12" s="6"/>
       <c r="E12" s="4"/>
       <c r="F12" s="6"/>
       <c r="G12" s="4"/>
     </row>
     <row r="13" spans="2:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="12" t="s">
         <v>0</v>
       </c>
       <c r="D13" s="1">
-        <v>59751</v>
+        <v>33314</v>
       </c>
       <c r="E13" s="3">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="F13" s="1">
-        <v>58416</v>
+        <v>52065</v>
       </c>
       <c r="G13" s="3">
-        <v>12</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="2:7" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="22"/>
-      <c r="C14" s="22"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
       <c r="D14" s="6"/>
       <c r="E14" s="4"/>
       <c r="F14" s="6"/>
       <c r="G14" s="4"/>
     </row>
     <row r="15" spans="2:7" ht="33" x14ac:dyDescent="0.25">
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="24" t="s">
+      <c r="C15" s="16" t="s">
         <v>10</v>
       </c>
       <c r="D15" s="1">
-        <v>193752</v>
+        <v>186539</v>
       </c>
       <c r="E15" s="3">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="F15" s="1">
-        <v>957811</v>
+        <v>866231</v>
       </c>
       <c r="G15" s="3">
-        <v>598</v>
+        <v>541</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added bombardier tool for load tests
</commit_message>
<xml_diff>
--- a/webservers/comparison.xlsx
+++ b/webservers/comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\github.com\gsainz\autocannon\webservers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D181679B-8E4D-4A62-870E-276B53E329D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB282E17-8BE7-4549-8FD2-881080952C5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{4D9F741E-112C-4F17-A62D-9BB75CA402CB}"/>
+    <workbookView xWindow="2655" yWindow="1485" windowWidth="21600" windowHeight="11505" xr2:uid="{4D9F741E-112C-4F17-A62D-9BB75CA402CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Web Servers" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>NODE</t>
   </si>
@@ -53,9 +53,6 @@
   </si>
   <si>
     <t>10 seconds - Pipelining 8</t>
-  </si>
-  <si>
-    <t>Server/Router</t>
   </si>
   <si>
     <t>Language</t>
@@ -69,10 +66,6 @@
   <si>
     <t>.NET Core 6.0
 (webapi)</t>
-  </si>
-  <si>
-    <t>AUTOCANNON 
-Load Tests</t>
   </si>
   <si>
     <t>Read (MB)</t>
@@ -181,6 +174,15 @@
       </rPr>
       <t>HTTP/1.1</t>
     </r>
+  </si>
+  <si>
+    <t>Server</t>
+  </si>
+  <si>
+    <t>Router</t>
+  </si>
+  <si>
+    <t>AUTOCANNON - TESTS</t>
   </si>
 </sst>
 </file>
@@ -254,7 +256,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -358,11 +360,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -388,9 +408,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="3" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -412,6 +429,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -427,10 +448,16 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -750,257 +777,270 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{140D5A91-2AEB-442F-9A05-CF626597CC11}">
-  <dimension ref="B2:G15"/>
+  <dimension ref="B2:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
-    <col min="3" max="3" width="31.28515625" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" style="7" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.42578125" style="7" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.28515625" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" style="7" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.42578125" style="7" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="21" t="s">
+    <row r="2" spans="2:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="23"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+    </row>
+    <row r="3" spans="2:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="25"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="21"/>
+    </row>
+    <row r="4" spans="2:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B5" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="14"/>
+      <c r="D5" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="1">
+        <v>233067</v>
+      </c>
+      <c r="F5" s="3">
+        <v>96</v>
+      </c>
+      <c r="G5" s="1">
+        <v>888242</v>
+      </c>
+      <c r="H5" s="3">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B6" s="19"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="9">
+        <v>270804</v>
+      </c>
+      <c r="F6" s="10">
+        <v>112</v>
+      </c>
+      <c r="G6" s="9">
+        <v>939506</v>
+      </c>
+      <c r="H6" s="10">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B7" s="19"/>
+      <c r="C7" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-    </row>
-    <row r="3" spans="2:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="23"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" s="20"/>
-    </row>
-    <row r="4" spans="2:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="8" t="s">
+      <c r="E7" s="2">
+        <v>241680</v>
+      </c>
+      <c r="F7" s="3">
+        <v>127</v>
+      </c>
+      <c r="G7" s="1">
+        <v>706845</v>
+      </c>
+      <c r="H7" s="3">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B8" s="19"/>
+      <c r="C8" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="11"/>
+      <c r="E8" s="1">
+        <v>262366</v>
+      </c>
+      <c r="F8" s="3">
+        <v>157</v>
+      </c>
+      <c r="G8" s="1">
+        <v>799248</v>
+      </c>
+      <c r="H8" s="3">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B9" s="19"/>
+      <c r="C9" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="1">
+        <v>249728</v>
+      </c>
+      <c r="F9" s="3">
+        <v>132</v>
+      </c>
+      <c r="G9" s="1">
+        <v>849918</v>
+      </c>
+      <c r="H9" s="3">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B10" s="19"/>
+      <c r="C10" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="17"/>
+      <c r="E10" s="1">
+        <v>577112</v>
+      </c>
+      <c r="F10" s="3">
+        <v>248</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1779269</v>
+      </c>
+      <c r="H10" s="3">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B11" s="20"/>
+      <c r="C11" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="9">
+        <v>554514</v>
+      </c>
+      <c r="F11" s="10">
+        <v>284</v>
+      </c>
+      <c r="G11" s="9">
+        <v>1571096</v>
+      </c>
+      <c r="H11" s="10">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" ht="3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1">
+        <v>33314</v>
+      </c>
+      <c r="F13" s="3">
+        <v>23</v>
+      </c>
+      <c r="G13" s="1">
+        <v>52065</v>
+      </c>
+      <c r="H13" s="3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="4"/>
+    </row>
+    <row r="15" spans="2:8" ht="33" x14ac:dyDescent="0.25">
+      <c r="B15" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="5" t="s">
+      <c r="C15" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B5" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="2">
-        <v>241680</v>
-      </c>
-      <c r="E5" s="3">
-        <v>127</v>
-      </c>
-      <c r="F5" s="1">
-        <v>706845</v>
-      </c>
-      <c r="G5" s="3">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B6" s="18"/>
-      <c r="C6" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="10">
-        <v>270804</v>
-      </c>
-      <c r="E6" s="11">
-        <v>112</v>
-      </c>
-      <c r="F6" s="10">
-        <v>939506</v>
-      </c>
-      <c r="G6" s="11">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B7" s="18"/>
-      <c r="C7" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="1">
-        <v>262366</v>
-      </c>
-      <c r="E7" s="3">
-        <v>157</v>
-      </c>
-      <c r="F7" s="1">
-        <v>743553</v>
-      </c>
-      <c r="G7" s="3">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B8" s="18"/>
-      <c r="C8" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="1">
-        <v>249728</v>
-      </c>
-      <c r="E8" s="3">
-        <v>132</v>
-      </c>
-      <c r="F8" s="1">
-        <v>849918</v>
-      </c>
-      <c r="G8" s="3">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B9" s="18"/>
-      <c r="C9" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="1">
-        <v>233067</v>
-      </c>
-      <c r="E9" s="3">
-        <v>96</v>
-      </c>
-      <c r="F9" s="1">
-        <v>888242</v>
-      </c>
-      <c r="G9" s="3">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B10" s="18"/>
-      <c r="C10" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="1">
-        <v>577112</v>
-      </c>
-      <c r="E10" s="3">
-        <v>248</v>
-      </c>
-      <c r="F10" s="1">
-        <v>1779269</v>
-      </c>
-      <c r="G10" s="3">
-        <v>765</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B11" s="19"/>
-      <c r="C11" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="10">
-        <v>554514</v>
-      </c>
-      <c r="E11" s="11">
-        <v>284</v>
-      </c>
-      <c r="F11" s="10">
-        <v>1571096</v>
-      </c>
-      <c r="G11" s="11">
-        <v>804</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" ht="3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="4"/>
-    </row>
-    <row r="13" spans="2:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="D13" s="1">
-        <v>33314</v>
-      </c>
-      <c r="E13" s="3">
-        <v>23</v>
-      </c>
-      <c r="F13" s="1">
-        <v>52065</v>
-      </c>
-      <c r="G13" s="3">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="4"/>
-    </row>
-    <row r="15" spans="2:7" ht="33" x14ac:dyDescent="0.25">
-      <c r="B15" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="1">
+      <c r="D15" s="17"/>
+      <c r="E15" s="1">
         <v>186539</v>
       </c>
-      <c r="E15" s="3">
+      <c r="F15" s="3">
         <v>116</v>
       </c>
-      <c r="F15" s="1">
+      <c r="G15" s="1">
         <v>866231</v>
       </c>
-      <c r="G15" s="3">
+      <c r="H15" s="3">
         <v>541</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="B5:B11"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="B2:D3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>